<commit_message>
I created summary tables
 I created summary tables based on threshold values for the research chapter, and extracted the API KEY from the chunkolasi_algoritmus_teszteles_mérés.py file, because I need to make it public on GitHub.
</commit_message>
<xml_diff>
--- a/chunkSizeTesting/ossz_0_65_5_kerdes.xlsx
+++ b/chunkSizeTesting/ossz_0_65_5_kerdes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krisztina_PC\flask-chatbot\chunkSizeTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A625B3-2803-4B9F-8C52-F5B6B7ABD46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C8141-BADE-440F-A3A0-7910F8419BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{78F2CBAC-EB64-40DA-A26A-4B58E3DB331A}"/>
   </bookViews>
@@ -38,16 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
-    <t>LLM model</t>
-  </si>
-  <si>
     <t>Chunk méret</t>
-  </si>
-  <si>
-    <t>Pontosság(%)</t>
-  </si>
-  <si>
-    <t>Átlagos feldolgozási idő</t>
   </si>
   <si>
     <t>Chunk (darab) száma</t>
@@ -66,6 +57,15 @@
   </si>
   <si>
     <t>text-embedding-3-large</t>
+  </si>
+  <si>
+    <t>Átlagos feldolgozási idő (s)</t>
+  </si>
+  <si>
+    <t>Pontosság (%)</t>
+  </si>
+  <si>
+    <t>LLM modell</t>
   </si>
 </sst>
 </file>
@@ -128,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -136,11 +136,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -478,7 +476,7 @@
   <dimension ref="B2:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,443 +485,444 @@
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
     <col min="4" max="4" width="18.109375" customWidth="1"/>
     <col min="5" max="5" width="32.33203125" customWidth="1"/>
-    <col min="6" max="6" width="32.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="C3" s="1">
         <v>256</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="1">
         <v>100</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="1">
         <v>1.365718078613281</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="1">
         <v>139</v>
       </c>
-      <c r="G3" s="5">
-        <v>0.65</v>
-      </c>
-      <c r="H3" s="5">
+      <c r="G3" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="H3" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
-        <v>7</v>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C4" s="2">
         <v>384</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>100</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.91391224861145015</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>101</v>
       </c>
-      <c r="G4" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="G4" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H4" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>7</v>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C5" s="2">
         <v>512</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>100</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>1.8619642734527591</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>83</v>
       </c>
-      <c r="G5" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="G5" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H5" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>7</v>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C6" s="2">
         <v>768</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>0.97137966156005862</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>66</v>
       </c>
-      <c r="G6" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H6" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>7</v>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C7" s="2">
         <v>1024</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>100</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>0.95285534858703613</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>61</v>
       </c>
-      <c r="G7" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="G7" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H7" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>7</v>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C8" s="2">
         <v>2048</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>100</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>1.876556301116943</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <v>52</v>
       </c>
-      <c r="G8" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="G8" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H8" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
-        <v>8</v>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>256</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="1">
         <v>60</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="1">
         <v>1.049689865112305</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="1">
         <v>139</v>
       </c>
-      <c r="G9" s="5">
-        <v>0.65</v>
-      </c>
-      <c r="H9" s="5">
+      <c r="G9" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="H9" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>8</v>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C10" s="2">
         <v>384</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>20</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>0.89921751022338869</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <v>101</v>
       </c>
-      <c r="G10" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="G10" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H10" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
-        <v>8</v>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C11" s="2">
         <v>512</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>40</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>1.0868830204010009</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <v>83</v>
       </c>
-      <c r="G11" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="G11" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H11" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>8</v>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C12" s="2">
         <v>768</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>20</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>0.91250677108764644</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>66</v>
       </c>
-      <c r="G12" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="G12" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H12" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C13" s="2">
         <v>1024</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>20</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>0.9084072589874268</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>61</v>
       </c>
-      <c r="G13" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="G13" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H13" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
-        <v>8</v>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C14" s="2">
         <v>2048</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>20</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>1.049073553085327</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>52</v>
       </c>
-      <c r="G14" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="G14" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H14" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
-        <v>9</v>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C15" s="1">
         <v>256</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="1">
         <v>60</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="1">
         <v>2.090820741653443</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="1">
         <v>139</v>
       </c>
-      <c r="G15" s="5">
-        <v>0.65</v>
-      </c>
-      <c r="H15" s="5">
+      <c r="G15" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="H15" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>9</v>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C16" s="2">
         <v>384</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>0</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>1.602821254730225</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>101</v>
       </c>
-      <c r="G16" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H16" s="3">
+      <c r="G16" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H16" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
-        <v>9</v>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C17" s="2">
         <v>512</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>20</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>1.578389263153076</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <v>83</v>
       </c>
-      <c r="G17" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H17" s="3">
+      <c r="G17" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H17" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>9</v>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C18" s="2">
         <v>768</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>0</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>1.8718407630920411</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <v>66</v>
       </c>
-      <c r="G18" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H18" s="3">
+      <c r="G18" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H18" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
-        <v>9</v>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="2">
         <v>1024</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>20</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>1.308083486557007</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>61</v>
       </c>
-      <c r="G19" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H19" s="3">
+      <c r="G19" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H19" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>9</v>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C20" s="2">
         <v>2048</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>0</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>1.516331338882446</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <v>52</v>
       </c>
-      <c r="G20" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="H20" s="3">
+      <c r="G20" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="H20" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>